<commit_message>
advanced tab and associated papers
</commit_message>
<xml_diff>
--- a/ScanningMethodOverview.xlsx
+++ b/ScanningMethodOverview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pauli\Desktop\PropellerProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CB9E346E-CA4E-4E4B-9439-BC336ABC18D4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4FD5CA96-8106-40DA-9DF1-09A2F5E400F4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="10988" xr2:uid="{9F5E1D82-68B1-40EE-8D92-600CFA77743C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>Scanning method overview</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>Domain</t>
-  </si>
-  <si>
-    <t>Very low</t>
   </si>
   <si>
     <t>+++</t>
@@ -73,38 +70,7 @@
 Fast</t>
   </si>
   <si>
-    <t xml:space="preserve">Reflective surface
-Sensitive to light </t>
-  </si>
-  <si>
     <t>0.1m to km</t>
-  </si>
-  <si>
-    <t>Very slow
-No complex shape</t>
-  </si>
-  <si>
-    <t>1micro
-submicro if blue LED</t>
-  </si>
-  <si>
-    <t>Max resolution</t>
-  </si>
-  <si>
-    <t>Micrometer</t>
-  </si>
-  <si>
-    <t>Depends on picture
-4/pixel</t>
-  </si>
-  <si>
-    <t>10micro</t>
-  </si>
-  <si>
-    <t>Low</t>
-  </si>
-  <si>
-    <t>Long (km)</t>
   </si>
   <si>
     <t>Application examples</t>
@@ -121,13 +87,6 @@
 Landslide Activity Analysis</t>
   </si>
   <si>
-    <t>Reflective surface
-Slow</t>
-  </si>
-  <si>
-    <t>Big object</t>
-  </si>
-  <si>
     <t>Motion friendly
 Fast</t>
   </si>
@@ -166,17 +125,79 @@
 Phase comparison</t>
   </si>
   <si>
+    <t>Reflective surface
+Expensive</t>
+  </si>
+  <si>
+    <t>2mm @30 m
+4mm @ 50 m
+7mm @ 100m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typical resolution </t>
+  </si>
+  <si>
+    <t>40-100 micro for range 15-45 cm</t>
+  </si>
+  <si>
+    <t>5-100 micro for range 5-150m
+submicro possible if blue LED</t>
+  </si>
+  <si>
+    <t>10cm - km</t>
+  </si>
+  <si>
+    <t>2cm - 150m</t>
+  </si>
+  <si>
+    <t>1m - km</t>
+  </si>
+  <si>
+    <t>In contact with probe</t>
+  </si>
+  <si>
+    <t>Fast</t>
+  </si>
+  <si>
+    <t>High quality scanning 
+Quality checking
+Reference Scanning</t>
+  </si>
+  <si>
+    <t>Depends on pictures
+Resolution = pixel/4</t>
+  </si>
+  <si>
+    <t>Pauline Ml</t>
+  </si>
+  <si>
     <t>3D shape scanning [138]
+Doc of Historic Buildings
 Translucent Object (Phase)
 Lidar</t>
   </si>
   <si>
+    <t>Terrestrial</t>
+  </si>
+  <si>
+    <t>Very slow
+No complex shape
+Stationary</t>
+  </si>
+  <si>
     <t>Reflective surface
+Sensitive to light 
+Stationary</t>
+  </si>
+  <si>
+    <t>Reflective surface
+Slow
+Stationary</t>
+  </si>
+  <si>
+    <t>Reflective surface
+Stationary
 Processing (computation time)</t>
-  </si>
-  <si>
-    <t>Reflective surface
-Expensive</t>
   </si>
 </sst>
 </file>
@@ -242,7 +263,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -315,11 +336,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -349,22 +379,25 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -683,12 +716,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FD21A0D-D8C0-470E-9545-9ADEBF26895A}">
   <dimension ref="B2:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22.06640625" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
+    <col min="1" max="1" width="6" customWidth="1"/>
+    <col min="4" max="4" width="25.3984375" customWidth="1"/>
     <col min="6" max="6" width="27.3984375" customWidth="1"/>
     <col min="7" max="7" width="26.3984375" customWidth="1"/>
   </cols>
@@ -713,15 +748,17 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="C5" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="15" t="s">
-        <v>38</v>
+      <c r="E5" s="11" t="s">
+        <v>26</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>6</v>
@@ -730,42 +767,44 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B6" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>21</v>
+        <v>29</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="27" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>16</v>
+      <c r="C7" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="27" customHeight="1" x14ac:dyDescent="0.5">
@@ -773,19 +812,19 @@
         <v>9</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.5">
@@ -793,19 +832,19 @@
         <v>10</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="58.9" customHeight="1" x14ac:dyDescent="0.5">
@@ -813,41 +852,47 @@
         <v>11</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="F10" s="9" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="58.15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="9"/>
+        <v>15</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="D11" s="9" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="27" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D12" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>35</v>
+      <c r="D12" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improved keep upper blade, need cutting plane
</commit_message>
<xml_diff>
--- a/ScanningMethodOverview.xlsx
+++ b/ScanningMethodOverview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pauli\Desktop\PropellerProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4FD5CA96-8106-40DA-9DF1-09A2F5E400F4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CD7AB599-B10C-4793-B7BE-AF14F2DF9D1E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="10988" xr2:uid="{9F5E1D82-68B1-40EE-8D92-600CFA77743C}"/>
   </bookViews>
@@ -716,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FD21A0D-D8C0-470E-9545-9ADEBF26895A}">
   <dimension ref="B2:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22.06640625" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -767,7 +767,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B6" s="10" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
added price to excel
</commit_message>
<xml_diff>
--- a/ScanningMethodOverview.xlsx
+++ b/ScanningMethodOverview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pauli\Desktop\PropellerProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CD7AB599-B10C-4793-B7BE-AF14F2DF9D1E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{89C84B5A-2595-44A4-B106-3A0C66F4A812}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="10988" xr2:uid="{9F5E1D82-68B1-40EE-8D92-600CFA77743C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="65">
   <si>
     <t>Scanning method overview</t>
   </si>
@@ -111,9 +111,6 @@
 Line detection and matching</t>
   </si>
   <si>
-    <t>Kinect ?</t>
-  </si>
-  <si>
     <t>Tool free calibration
 Scanning of architecture elements</t>
   </si>
@@ -156,9 +153,6 @@
     <t>In contact with probe</t>
   </si>
   <si>
-    <t>Fast</t>
-  </si>
-  <si>
     <t>High quality scanning 
 Quality checking
 Reference Scanning</t>
@@ -168,36 +162,101 @@
 Resolution = pixel/4</t>
   </si>
   <si>
-    <t>Pauline Ml</t>
+    <t>Terrestrial</t>
+  </si>
+  <si>
+    <t>Very slow
+No complex shape
+Stationary</t>
+  </si>
+  <si>
+    <t>Reflective surface
+Sensitive to light 
+Stationary</t>
+  </si>
+  <si>
+    <t>Reflective surface
+Slow
+Stationary</t>
+  </si>
+  <si>
+    <t>Reflective surface
+Stationary
+Processing (computation time)</t>
   </si>
   <si>
     <t>3D shape scanning [138]
 Doc of Historic Buildings
 Translucent Object (Phase)
-Lidar</t>
-  </si>
-  <si>
-    <t>Terrestrial</t>
-  </si>
-  <si>
-    <t>Very slow
-No complex shape
-Stationary</t>
-  </si>
-  <si>
-    <t>Reflective surface
-Sensitive to light 
-Stationary</t>
-  </si>
-  <si>
-    <t>Reflective surface
-Slow
-Stationary</t>
-  </si>
-  <si>
-    <t>Reflective surface
-Stationary
-Processing (computation time)</t>
+Lidar - Kinect</t>
+  </si>
+  <si>
+    <t>Price (@50micro)</t>
+  </si>
+  <si>
+    <t>Fast
+Can capture textures and colors</t>
+  </si>
+  <si>
+    <t>space spider (0.05mm): https://www.artec3d.com/portable-3d-scanners/artec-spider#specifications</t>
+  </si>
+  <si>
+    <t>Shining3d scanner DS-300</t>
+  </si>
+  <si>
+    <t>23'000CHF</t>
+  </si>
+  <si>
+    <t>10'000CHF + 5000CHF (software)</t>
+  </si>
+  <si>
+    <t>structured light</t>
+  </si>
+  <si>
+    <t>Wireless freescan X7 + Shining 3D</t>
+  </si>
+  <si>
+    <t>laser triang</t>
+  </si>
+  <si>
+    <t>20'000-50'000Chf</t>
+  </si>
+  <si>
+    <t>D2000 3Shape</t>
+  </si>
+  <si>
+    <t>5micron</t>
+  </si>
+  <si>
+    <t>&lt;10 micron</t>
+  </si>
+  <si>
+    <t>50 micron</t>
+  </si>
+  <si>
+    <t>Handyscan 700 Creaform</t>
+  </si>
+  <si>
+    <t>50'000-100'000CHF</t>
+  </si>
+  <si>
+    <t>15'000 CHF</t>
+  </si>
+  <si>
+    <t>50'000CHF</t>
+  </si>
+  <si>
+    <t>5'000CHF (camera)</t>
+  </si>
+  <si>
+    <t>50 micro not possible</t>
+  </si>
+  <si>
+    <t>Metrascan 350 elite
+https://www.creaform3d.com/en/metrology-solutions/optical-3d-scanner-metrascan</t>
+  </si>
+  <si>
+    <t>150'000CHF</t>
   </si>
 </sst>
 </file>
@@ -349,7 +408,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -398,6 +457,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -714,16 +785,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FD21A0D-D8C0-470E-9545-9ADEBF26895A}">
-  <dimension ref="B2:G12"/>
+  <dimension ref="B2:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22.06640625" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
     <col min="4" max="4" width="25.3984375" customWidth="1"/>
+    <col min="5" max="5" width="25.73046875" customWidth="1"/>
     <col min="6" max="6" width="27.3984375" customWidth="1"/>
     <col min="7" max="7" width="26.3984375" customWidth="1"/>
   </cols>
@@ -748,9 +820,7 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B5" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="B5" s="1"/>
       <c r="C5" s="7" t="s">
         <v>3</v>
       </c>
@@ -758,7 +828,7 @@
         <v>4</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>6</v>
@@ -769,130 +839,221 @@
     </row>
     <row r="6" spans="2:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B6" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="27" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>14</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B7" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="27" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="31.9" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D9" s="9" t="s">
         <v>13</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>43</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>44</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="G9" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="44.25" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="58.9" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="58.15" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="27" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+    </row>
+    <row r="14" spans="2:7" ht="27" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B14" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="18" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="10" spans="2:7" ht="58.9" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" ht="58.15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="27" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D12" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>23</v>
+      <c r="D14" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="27" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B15" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="27" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B16" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="27" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B17" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="27" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B18" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="27" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B19" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>